<commit_message>
Updated llbv3 bill of materials
</commit_message>
<xml_diff>
--- a/Electronics/Low Level/BoM.xlsx
+++ b/Electronics/Low Level/BoM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level v3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Projects/elcano/Electronics/Low Level/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9817737A-49D1-8948-890E-72CDF67D6874}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606861FC-6D11-DC42-BDC5-45C7AFCBA84C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21160" xr2:uid="{F66CC82F-6637-7D48-A4BB-0FCD493187ED}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="199">
   <si>
     <t>Qty</t>
   </si>
@@ -224,9 +224,6 @@
     <t>10k</t>
   </si>
   <si>
-    <t>R11, R12, R15, R16</t>
-  </si>
-  <si>
     <t>R10</t>
   </si>
   <si>
@@ -332,15 +329,6 @@
     <t>R1, R2, R3, R4, R9, R17</t>
   </si>
   <si>
-    <t>5-104069-4</t>
-  </si>
-  <si>
-    <t>CONN_5-104069-4_TYCO</t>
-  </si>
-  <si>
-    <t>STEERING_IO</t>
-  </si>
-  <si>
     <t>560pF</t>
   </si>
   <si>
@@ -617,9 +605,6 @@
     <t>2N3904-APCT-ND</t>
   </si>
   <si>
-    <t>A107254-ND</t>
-  </si>
-  <si>
     <t>102-1153-ND</t>
   </si>
   <si>
@@ -663,6 +648,21 @@
   </si>
   <si>
     <t>‎MJ1-2503A‎</t>
+  </si>
+  <si>
+    <t>RJ45-8L-B</t>
+  </si>
+  <si>
+    <t>Steering Header</t>
+  </si>
+  <si>
+    <t>Modular jack for steering peripherals</t>
+  </si>
+  <si>
+    <t>RJ45 8 pin jack</t>
+  </si>
+  <si>
+    <t>R12, R15, R16</t>
   </si>
 </sst>
 </file>
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A12E2CF-710F-D148-A35C-437BFC6C6DF7}">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="141" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1102,22 +1102,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -1170,16 +1170,16 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
@@ -1199,19 +1199,19 @@
         <v>43</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H3" t="s">
         <v>46</v>
@@ -1225,19 +1225,19 @@
         <v>43</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F4" t="s">
         <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
         <v>46</v>
@@ -1254,10 +1254,10 @@
         <v>42</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F5" t="s">
         <v>44</v>
@@ -1271,25 +1271,25 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F6" t="s">
         <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H6" t="s">
         <v>46</v>
@@ -1306,10 +1306,10 @@
         <v>100</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
         <v>48</v>
@@ -1323,25 +1323,25 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F8" t="s">
         <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H8" t="s">
         <v>50</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>47</v>
@@ -1358,16 +1358,16 @@
         <v>51</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F9" t="s">
         <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>198</v>
       </c>
       <c r="H9" t="s">
         <v>50</v>
@@ -1384,16 +1384,16 @@
         <v>120</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F10" t="s">
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
         <v>50</v>
@@ -1401,25 +1401,25 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F11" t="s">
         <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
         <v>50</v>
@@ -1433,19 +1433,19 @@
         <v>47</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F12" t="s">
         <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H12" t="s">
         <v>50</v>
@@ -1456,46 +1456,46 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" t="s">
-        <v>61</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="R13" t="s">
         <v>62</v>
       </c>
-      <c r="N13" t="s">
-        <v>55</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="U13" t="s">
         <v>63</v>
-      </c>
-      <c r="U13" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -1503,25 +1503,25 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F14" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>68</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>69</v>
-      </c>
-      <c r="H14" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -1529,25 +1529,25 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F15" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>72</v>
       </c>
-      <c r="G15" t="s">
-        <v>73</v>
-      </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
@@ -1555,162 +1555,162 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" t="s">
         <v>77</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F16" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" t="s">
-        <v>78</v>
       </c>
       <c r="L16">
         <v>2845124</v>
       </c>
       <c r="W16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F17" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>81</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>82</v>
       </c>
-      <c r="H17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" t="s">
+        <v>98</v>
+      </c>
+      <c r="S18" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="T18" t="s">
         <v>100</v>
       </c>
-      <c r="G18" t="s">
-        <v>101</v>
-      </c>
-      <c r="H18" t="s">
-        <v>102</v>
-      </c>
-      <c r="S18" t="s">
-        <v>103</v>
-      </c>
-      <c r="T18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19" t="s">
+        <v>147</v>
+      </c>
+      <c r="H19" t="s">
+        <v>148</v>
+      </c>
+      <c r="I19" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="J19" t="s">
+        <v>150</v>
+      </c>
+      <c r="K19" t="s">
+        <v>151</v>
+      </c>
+      <c r="M19" t="s">
+        <v>152</v>
+      </c>
+      <c r="N19" t="s">
+        <v>145</v>
+      </c>
+      <c r="R19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
         <v>154</v>
       </c>
-      <c r="F19" t="s">
-        <v>150</v>
-      </c>
-      <c r="G19" t="s">
-        <v>151</v>
-      </c>
-      <c r="H19" t="s">
-        <v>152</v>
-      </c>
-      <c r="I19" t="s">
-        <v>153</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="C20" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="K19" t="s">
+      <c r="D20" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" t="s">
         <v>155</v>
       </c>
-      <c r="M19" t="s">
+      <c r="G20" t="s">
         <v>156</v>
       </c>
-      <c r="N19" t="s">
-        <v>149</v>
-      </c>
-      <c r="R19" t="s">
+      <c r="H20" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="U20" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E20" t="s">
-        <v>167</v>
-      </c>
-      <c r="F20" t="s">
-        <v>159</v>
-      </c>
-      <c r="G20" t="s">
-        <v>160</v>
-      </c>
-      <c r="H20" t="s">
-        <v>161</v>
-      </c>
-      <c r="U20" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1721,10 +1721,10 @@
         <v>35</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F21" t="s">
         <v>37</v>
@@ -1745,94 +1745,94 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F22" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="U22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="C24" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F24" t="s">
         <v>135</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>136</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="S24" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="T24" t="s">
         <v>139</v>
       </c>
-      <c r="G24" t="s">
-        <v>140</v>
-      </c>
-      <c r="H24" t="s">
-        <v>141</v>
-      </c>
-      <c r="S24" t="s">
-        <v>142</v>
-      </c>
-      <c r="T24" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1840,10 +1840,10 @@
         <v>19</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
@@ -1861,123 +1861,112 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>197</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F26" t="s">
-        <v>89</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="E26" s="2"/>
       <c r="G26" t="s">
-        <v>90</v>
-      </c>
-      <c r="L26">
-        <v>51040694</v>
-      </c>
-      <c r="W26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+      <c r="H26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F27" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H27" t="s">
+        <v>108</v>
+      </c>
+      <c r="S27" t="s">
         <v>109</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F27" t="s">
-        <v>110</v>
-      </c>
-      <c r="G27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H27" t="s">
-        <v>112</v>
-      </c>
-      <c r="S27" t="s">
-        <v>113</v>
       </c>
       <c r="U27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G28" t="s">
+        <v>142</v>
+      </c>
+      <c r="H28" t="s">
+        <v>143</v>
+      </c>
+      <c r="P28" t="s">
         <v>144</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F28" t="s">
-        <v>145</v>
-      </c>
-      <c r="G28" t="s">
-        <v>146</v>
-      </c>
-      <c r="H28" t="s">
-        <v>147</v>
-      </c>
-      <c r="P28" t="s">
-        <v>148</v>
-      </c>
       <c r="Q28" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F29" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1994,7 +1983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2016,16 +2005,16 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F33" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G33" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H33" t="s">
         <v>31</v>
@@ -2036,16 +2025,16 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G34" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H34" t="s">
         <v>31</v>
@@ -2056,16 +2045,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F35" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G35" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H35" t="s">
         <v>31</v>
@@ -2076,16 +2065,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F36" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G36" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H36" t="s">
         <v>31</v>
@@ -2096,16 +2085,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" t="s">
         <v>94</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F37" t="s">
-        <v>95</v>
-      </c>
-      <c r="G37" t="s">
-        <v>98</v>
       </c>
       <c r="H37" t="s">
         <v>31</v>
@@ -2116,16 +2105,16 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F38" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G38" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H38" t="s">
         <v>31</v>
@@ -2136,16 +2125,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F39" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G39" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H39" t="s">
         <v>31</v>

</xml_diff>